<commit_message>
Added new v5 code changes
</commit_message>
<xml_diff>
--- a/data/Extracted_Data.xlsx
+++ b/data/Extracted_Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://airtcom-my.sharepoint.com/personal/rbaldania_randomtrees_com/Documents/Rachana_Code/ETRM_AI_Matching_RB/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{9DEC4CDC-7B9D-4D6A-BDDB-EF6975189794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{35A7EA6C-9D83-4FED-835D-6AE9034D785C}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{9DEC4CDC-7B9D-4D6A-BDDB-EF6975189794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A6300C27-6A25-439F-BB8B-3137DE16D4EC}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="62">
   <si>
     <t xml:space="preserve">Pdf file name </t>
   </si>
@@ -1500,6 +1500,49 @@
   <si>
     <t>60625 JAYHAWK, NV</t>
   </si>
+  <si>
+    <t>Download
+{
+  "extracted_name": "Butane",
+  "matched_name": "Butane",
+  "matching_score": 1,
+  "reason": "Exact name match",
+  "etrm_code": "400007248.0",
+  "etrm_id": "1560",
+  "alternatives": [
+    {
+      "matched_name": "BUTANE/BUTLYENE SALES",
+      "score": 0.8,
+      "code": "400007558.0",
+      "id": "2251"
+    },
+    {
+      "matched_name": "Normal Butane Frac",
+      "score": 0.8,
+      "code": "400007561.0",
+      "id": "2180"
+    },
+    {
+      "matched_name": "Refridg Normal Butane",
+      "score": 0.8,
+      "code": "400007562.0",
+      "id": "2071"
+    },
+    {
+      "matched_name": "Cap and Trade Butane Obligations Quebec",
+      "score": 0.8,
+      "code": null,
+      "id": "2691"
+    },
+    {
+      "matched_name": "Cap and Trade Butane Potential Obligations Quebec",
+      "score": 0.8,
+      "code": null,
+      "id": "2692"
+    }
+  ]
+}</t>
+  </si>
 </sst>
 </file>
 
@@ -1554,7 +1597,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1567,6 +1610,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1906,19 +1952,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63054F5F-1F03-495C-9984-59C4C2B3D891}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="42" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="42" style="4"/>
     <col min="3" max="3" width="42" style="2"/>
+    <col min="7" max="7" width="82.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1938,7 +1985,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1958,7 +2005,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1978,7 +2025,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1998,7 +2045,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2018,7 +2065,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -2038,7 +2085,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -2058,7 +2105,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -2078,7 +2125,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="408.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -2097,8 +2144,11 @@
       <c r="F9" t="s">
         <v>48</v>
       </c>
+      <c r="G9" s="7" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="10" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>49</v>
       </c>
@@ -2118,7 +2168,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>51</v>
       </c>
@@ -2138,7 +2188,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>57</v>
       </c>

</xml_diff>